<commit_message>
Fix target duration | Add checks to analysis and late_res, slow_mvmnt | Fix missing data test
New checks analysis: late res, slow mvmnt, early start, incorrect ans.
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/code/Code_Output_Explanation.xlsx
+++ b/experiment/RUN_ME/code/Code_Output_Explanation.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\experiment\RUN_ME\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC8456C-9145-444D-A985-FD33D247A276}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
   <si>
     <t>prime</t>
   </si>
@@ -323,12 +322,24 @@
   </si>
   <si>
     <t>Indicates this is a practice trial.</t>
+  </si>
+  <si>
+    <t>late_res</t>
+  </si>
+  <si>
+    <t>slow_mvmnt</t>
+  </si>
+  <si>
+    <t>subject started moving too late.</t>
+  </si>
+  <si>
+    <t>movement was too slow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -643,16 +654,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BH3" sqref="BH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:58" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -827,8 +838,14 @@
       <c r="BF1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="BG1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:58" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
@@ -995,6 +1012,12 @@
         <v>12</v>
       </c>
       <c r="BF2" s="1"/>
+      <c r="BG2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 'early_res' and 'incorrect' to experiment and analysis
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/code/Code_Output_Explanation.xlsx
+++ b/experiment/RUN_ME/code/Code_Output_Explanation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\experiment\RUN_ME\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BE7E97-27C4-43DF-8FA0-C543FA88D06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
   <si>
     <t>prime</t>
   </si>
@@ -334,12 +335,18 @@
   </si>
   <si>
     <t>movement was too slow</t>
+  </si>
+  <si>
+    <t>early_res</t>
+  </si>
+  <si>
+    <t>subject started moving too early.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -654,16 +661,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BH3" sqref="BH3"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BI3" sqref="BI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:60" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -844,8 +851,11 @@
       <c r="BH1" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="BI1" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="2" spans="1:60" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
@@ -1017,6 +1027,9 @@
       </c>
       <c r="BH2" s="1" t="s">
         <v>102</v>
+      </c>
+      <c r="BI2" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trials to quitters |  p.DAY in names | MAD, Traj formating | Fix subscreen
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/code/Code_Output_Explanation.xlsx
+++ b/experiment/RUN_ME/code/Code_Output_Explanation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BE7E97-27C4-43DF-8FA0-C543FA88D06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E93BD2C-DB81-422E-B0DC-A198934968BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="107">
   <si>
     <t>prime</t>
   </si>
@@ -341,6 +341,12 @@
   </si>
   <si>
     <t>subject started moving too early.</t>
+  </si>
+  <si>
+    <t>quit</t>
+  </si>
+  <si>
+    <t>sub quit the experiment before reaching this trial</t>
   </si>
 </sst>
 </file>
@@ -662,15 +668,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI2"/>
+  <dimension ref="A1:BJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BI3" sqref="BI3"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BJ3" sqref="BJ3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.19921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:61" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:62" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -854,8 +860,11 @@
       <c r="BI1" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="BJ1" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="2" spans="1:61" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:62" ht="69" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
@@ -1030,6 +1039,9 @@
       </c>
       <c r="BI2" s="1" t="s">
         <v>104</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
written that same means congruent.
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/code/Code_Output_Explanation.xlsx
+++ b/experiment/RUN_ME/code/Code_Output_Explanation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E93BD2C-DB81-422E-B0DC-A198934968BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8021E170-B71A-482C-B6DB-935D1B90E083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>prime is on the left (1) / right (0) on recognition task</t>
   </si>
   <si>
-    <t>prime-target relation: same word(1) / different word(0)</t>
-  </si>
-  <si>
     <t>natural_left</t>
   </si>
   <si>
@@ -310,43 +307,46 @@
     <t>iBlock</t>
   </si>
   <si>
+    <t>list_id</t>
+  </si>
+  <si>
+    <t>Name of trials list used for this subject</t>
+  </si>
+  <si>
+    <t>practice</t>
+  </si>
+  <si>
+    <t>Indicates this is a practice trial.</t>
+  </si>
+  <si>
+    <t>late_res</t>
+  </si>
+  <si>
+    <t>slow_mvmnt</t>
+  </si>
+  <si>
+    <t>subject started moving too late.</t>
+  </si>
+  <si>
+    <t>movement was too slow</t>
+  </si>
+  <si>
+    <t>early_res</t>
+  </si>
+  <si>
+    <t>subject started moving too early.</t>
+  </si>
+  <si>
+    <t>quit</t>
+  </si>
+  <si>
+    <t>sub quit the experiment before reaching this trial</t>
+  </si>
+  <si>
+    <t>prime-target relation: same word=congruent=(1) / different word=incongruent=(0)</t>
+  </si>
+  <si>
     <t>same</t>
-  </si>
-  <si>
-    <t>list_id</t>
-  </si>
-  <si>
-    <t>Name of trials list used for this subject</t>
-  </si>
-  <si>
-    <t>practice</t>
-  </si>
-  <si>
-    <t>Indicates this is a practice trial.</t>
-  </si>
-  <si>
-    <t>late_res</t>
-  </si>
-  <si>
-    <t>slow_mvmnt</t>
-  </si>
-  <si>
-    <t>subject started moving too late.</t>
-  </si>
-  <si>
-    <t>movement was too slow</t>
-  </si>
-  <si>
-    <t>early_res</t>
-  </si>
-  <si>
-    <t>subject started moving too early.</t>
-  </si>
-  <si>
-    <t>quit</t>
-  </si>
-  <si>
-    <t>sub quit the experiment before reaching this trial</t>
   </si>
 </sst>
 </file>
@@ -670,39 +670,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BJ3" sqref="BJ3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.19921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.1875" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:62" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" ht="27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>16</v>
@@ -711,37 +711,37 @@
         <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="Q1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>1</v>
@@ -756,94 +756,94 @@
         <v>3</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="AC1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="AF1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="AI1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AJ1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="AN1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AO1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AP1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AR1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AY1" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="AZ1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>5</v>
@@ -852,21 +852,21 @@
         <v>6</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="BI1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BJ1" s="1" t="s">
-        <v>105</v>
-      </c>
     </row>
-    <row r="2" spans="1:62" ht="69" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" ht="81" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
@@ -875,43 +875,43 @@
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>8</v>
@@ -923,106 +923,106 @@
         <v>10</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="Y2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="AF2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AI2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AM2" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="AN2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AR2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AT2" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AU2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AV2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AY2" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="AZ2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BB2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BD2" s="1" t="s">
         <v>11</v>
@@ -1032,16 +1032,16 @@
       </c>
       <c r="BF2" s="1"/>
       <c r="BG2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="BH2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BI2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>